<commit_message>
Updated Analyses - Updated README
</commit_message>
<xml_diff>
--- a/project_sql/Data Analyses/2_top_paying_jobs_skills_insights.xlsx
+++ b/project_sql/Data Analyses/2_top_paying_jobs_skills_insights.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blnor\Downloads\Brennan\SQL for Data Analytics\SQL_Project_Data_Job_Analysis\project_sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blnor\Downloads\Brennan\SQL for Data Analytics\SQL_Project_Data_Job_Analysis\project_sql\Data Analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80842C9-2431-4EA9-AF52-B9CACDF5F5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBE186-7980-42D7-8FAD-573D74E8F642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2867,7 +2867,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,7 +3304,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="2">
-        <f>COUNTIFS($E$2:$E$67,G2)</f>
+        <f t="shared" ref="H2:H29" si="0">COUNTIFS($E$2:$E$67,G2)</f>
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -3334,7 +3334,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="1">
-        <f>COUNTIFS($E$2:$E$67,G3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -3364,7 +3364,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="1">
-        <f>COUNTIFS($E$2:$E$67,G4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -3394,7 +3394,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="1">
-        <f>COUNTIFS($E$2:$E$67,G5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -3424,7 +3424,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="1">
-        <f>COUNTIFS($E$2:$E$67,G6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -3454,7 +3454,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="1">
-        <f>COUNTIFS($E$2:$E$67,G7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -3484,7 +3484,7 @@
         <v>27</v>
       </c>
       <c r="H8" s="1">
-        <f>COUNTIFS($E$2:$E$67,G8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -3514,7 +3514,7 @@
         <v>36</v>
       </c>
       <c r="H9" s="1">
-        <f>COUNTIFS($E$2:$E$67,G9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3538,7 +3538,7 @@
         <v>37</v>
       </c>
       <c r="H10" s="1">
-        <f>COUNTIFS($E$2:$E$67,G10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3562,7 +3562,7 @@
         <v>44</v>
       </c>
       <c r="H11" s="1">
-        <f>COUNTIFS($E$2:$E$67,G11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3586,7 +3586,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="1">
-        <f>COUNTIFS($E$2:$E$67,G12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3610,7 +3610,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="1">
-        <f>COUNTIFS($E$2:$E$67,G13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3634,7 +3634,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="1">
-        <f>COUNTIFS($E$2:$E$67,G14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3658,7 +3658,7 @@
         <v>26</v>
       </c>
       <c r="H15" s="1">
-        <f>COUNTIFS($E$2:$E$67,G15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3682,7 +3682,7 @@
         <v>30</v>
       </c>
       <c r="H16" s="1">
-        <f>COUNTIFS($E$2:$E$67,G16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
         <v>32</v>
       </c>
       <c r="H17" s="1">
-        <f>COUNTIFS($E$2:$E$67,G17)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3730,7 +3730,7 @@
         <v>33</v>
       </c>
       <c r="H18" s="1">
-        <f>COUNTIFS($E$2:$E$67,G18)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3754,7 +3754,7 @@
         <v>38</v>
       </c>
       <c r="H19" s="1">
-        <f>COUNTIFS($E$2:$E$67,G19)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3778,7 +3778,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="1">
-        <f>COUNTIFS($E$2:$E$67,G20)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3802,7 +3802,7 @@
         <v>40</v>
       </c>
       <c r="H21" s="1">
-        <f>COUNTIFS($E$2:$E$67,G21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
         <v>41</v>
       </c>
       <c r="H22" s="1">
-        <f>COUNTIFS($E$2:$E$67,G22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3850,7 +3850,7 @@
         <v>13</v>
       </c>
       <c r="H23" s="1">
-        <f>COUNTIFS($E$2:$E$67,G23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -3874,7 +3874,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="1">
-        <f>COUNTIFS($E$2:$E$67,G24)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -3898,7 +3898,7 @@
         <v>31</v>
       </c>
       <c r="H25" s="1">
-        <f>COUNTIFS($E$2:$E$67,G25)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -3922,7 +3922,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="1">
-        <f>COUNTIFS($E$2:$E$67,G26)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -3946,7 +3946,7 @@
         <v>17</v>
       </c>
       <c r="H27" s="1">
-        <f>COUNTIFS($E$2:$E$67,G27)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -3970,7 +3970,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="1">
-        <f>COUNTIFS($E$2:$E$67,G28)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -3994,7 +3994,7 @@
         <v>7</v>
       </c>
       <c r="H29" s="1">
-        <f>COUNTIFS($E$2:$E$67,G29)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Big Updates to Query 5
</commit_message>
<xml_diff>
--- a/project_sql/Data Analyses/2_top_paying_jobs_skills_insights.xlsx
+++ b/project_sql/Data Analyses/2_top_paying_jobs_skills_insights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blnor\Downloads\Brennan\SQL for Data Analytics\SQL_Project_Data_Job_Analysis\project_sql\Data Analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBE186-7980-42D7-8FAD-573D74E8F642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B879957C-045A-4F69-BCEC-3EB7517F16CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="51">
   <si>
     <t>job_id</t>
   </si>
@@ -2864,11 +2864,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B29316-F211-4A02-938B-4209C4F5FF53}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3223,6 +3221,71 @@
       <c r="C30" s="5">
         <f t="shared" si="0"/>
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3239,7 +3302,7 @@
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K8"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>